<commit_message>
new branch edge for edge execution
</commit_message>
<xml_diff>
--- a/CucumberOK/Default.xlsx
+++ b/CucumberOK/Default.xlsx
@@ -470,7 +470,9 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>

</xml_diff>